<commit_message>
-Arreglos y cambios en el manual de usuario.
</commit_message>
<xml_diff>
--- a/Documentación/Casos de prueba.xlsx
+++ b/Documentación/Casos de prueba.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="106">
   <si>
     <t>Certficados</t>
   </si>
@@ -331,13 +331,16 @@
   </si>
   <si>
     <t>El administrador seleccionó en adopción y selecciona la opción de evaluar al adoptante</t>
+  </si>
+  <si>
+    <t>Certificado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,6 +365,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -603,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -636,54 +647,55 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -990,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52:D52"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43:F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1044,7 @@
       </c>
       <c r="H3" s="4">
         <f>COUNTIF(F9:F58, "Certificado")</f>
-        <v>0</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1050,7 +1062,7 @@
       </c>
       <c r="H4" s="3">
         <f>COUNTIF(F9:F58, "Pendiente")</f>
-        <v>50</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1119,7 +1131,7 @@
         <v>79</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -1135,7 +1147,7 @@
         <v>16</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1150,7 +1162,7 @@
         <v>18</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1165,7 +1177,7 @@
         <v>19</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1180,7 +1192,7 @@
         <v>83</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1195,7 +1207,7 @@
         <v>82</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1210,7 +1222,7 @@
         <v>82</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1225,7 +1237,7 @@
         <v>20</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1240,7 +1252,7 @@
         <v>22</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -1255,7 +1267,7 @@
         <v>24</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -1270,7 +1282,7 @@
         <v>26</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1285,17 +1297,17 @@
         <v>21</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="12">
         <v>13</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="21"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="13" t="s">
         <v>27</v>
       </c>
@@ -1307,130 +1319,130 @@
       <c r="B22" s="12">
         <v>14</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="21"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="13" t="s">
         <v>28</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>15</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="21"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="13" t="s">
         <v>29</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>16</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="21"/>
+      <c r="D24" s="23"/>
       <c r="E24" s="13" t="s">
         <v>33</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="12">
         <v>17</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="21"/>
+      <c r="D25" s="23"/>
       <c r="E25" s="13" t="s">
         <v>88</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="12">
         <v>18</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="21"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="13" t="s">
         <v>90</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="12">
         <v>19</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="D27" s="21"/>
+      <c r="D27" s="23"/>
       <c r="E27" s="13" t="s">
         <v>34</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="12">
         <v>20</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="21"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="13" t="s">
         <v>92</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="12">
         <v>21</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="22"/>
+      <c r="D29" s="34"/>
       <c r="E29" s="13" t="s">
         <v>35</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="12">
         <v>22</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="D30" s="21"/>
+      <c r="D30" s="23"/>
       <c r="E30" s="13" t="s">
         <v>37</v>
       </c>
@@ -1442,90 +1454,90 @@
       <c r="B31" s="12">
         <v>23</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="21"/>
+      <c r="D31" s="23"/>
       <c r="E31" s="15" t="s">
         <v>94</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="12">
         <v>24</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="21"/>
+      <c r="D32" s="23"/>
       <c r="E32" s="15" t="s">
         <v>95</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="12">
         <v>25</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="21"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="15" t="s">
         <v>96</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" s="12">
         <v>26</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="21"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="15" t="s">
         <v>42</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="12">
         <v>27</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="21"/>
+      <c r="D35" s="23"/>
       <c r="E35" s="15" t="s">
         <v>46</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" s="12">
         <v>28</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="21"/>
+      <c r="D36" s="23"/>
       <c r="E36" s="15" t="s">
         <v>78</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1533,15 +1545,15 @@
       <c r="B37" s="12">
         <v>29</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="21"/>
+      <c r="D37" s="23"/>
       <c r="E37" s="13" t="s">
         <v>51</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1549,15 +1561,15 @@
       <c r="B38" s="12">
         <v>30</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D38" s="21"/>
+      <c r="D38" s="23"/>
       <c r="E38" s="13" t="s">
         <v>26</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1565,15 +1577,15 @@
       <c r="B39" s="12">
         <v>31</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D39" s="21"/>
+      <c r="D39" s="23"/>
       <c r="E39" s="13" t="s">
         <v>21</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1581,15 +1593,15 @@
       <c r="B40" s="12">
         <v>32</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="D40" s="21"/>
+      <c r="D40" s="23"/>
       <c r="E40" s="13" t="s">
         <v>55</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1597,10 +1609,10 @@
       <c r="B41" s="12">
         <v>33</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="21"/>
+      <c r="D41" s="23"/>
       <c r="E41" s="13" t="s">
         <v>57</v>
       </c>
@@ -1613,10 +1625,10 @@
       <c r="B42" s="12">
         <v>34</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D42" s="21"/>
+      <c r="D42" s="23"/>
       <c r="E42" s="13" t="s">
         <v>59</v>
       </c>
@@ -1629,15 +1641,15 @@
       <c r="B43" s="12">
         <v>35</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="21"/>
+      <c r="D43" s="23"/>
       <c r="E43" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F43" s="14" t="s">
-        <v>10</v>
+      <c r="F43" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1645,15 +1657,15 @@
       <c r="B44" s="12">
         <v>36</v>
       </c>
-      <c r="C44" s="20" t="s">
+      <c r="C44" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D44" s="21"/>
+      <c r="D44" s="23"/>
       <c r="E44" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F44" s="14" t="s">
-        <v>10</v>
+      <c r="F44" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1661,15 +1673,15 @@
       <c r="B45" s="12">
         <v>37</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C45" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D45" s="21"/>
+      <c r="D45" s="23"/>
       <c r="E45" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="F45" s="14" t="s">
-        <v>10</v>
+      <c r="F45" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1677,15 +1689,15 @@
       <c r="B46" s="12">
         <v>38</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D46" s="21"/>
+      <c r="D46" s="23"/>
       <c r="E46" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F46" s="14" t="s">
-        <v>10</v>
+      <c r="F46" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1693,15 +1705,15 @@
       <c r="B47" s="12">
         <v>39</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="D47" s="21"/>
+      <c r="D47" s="23"/>
       <c r="E47" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F47" s="14" t="s">
-        <v>10</v>
+      <c r="F47" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1709,15 +1721,15 @@
       <c r="B48" s="12">
         <v>40</v>
       </c>
-      <c r="C48" s="20" t="s">
+      <c r="C48" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="D48" s="21"/>
+      <c r="D48" s="23"/>
       <c r="E48" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F48" s="14" t="s">
-        <v>10</v>
+      <c r="F48" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1725,15 +1737,15 @@
       <c r="B49" s="12">
         <v>41</v>
       </c>
-      <c r="C49" s="20" t="s">
+      <c r="C49" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="D49" s="21"/>
+      <c r="D49" s="23"/>
       <c r="E49" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="F49" s="14" t="s">
-        <v>10</v>
+      <c r="F49" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1741,15 +1753,15 @@
       <c r="B50" s="12">
         <v>42</v>
       </c>
-      <c r="C50" s="20" t="s">
+      <c r="C50" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D50" s="21"/>
+      <c r="D50" s="23"/>
       <c r="E50" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F50" s="14" t="s">
-        <v>10</v>
+      <c r="F50" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1757,15 +1769,15 @@
       <c r="B51" s="12">
         <v>43</v>
       </c>
-      <c r="C51" s="20" t="s">
+      <c r="C51" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="D51" s="22"/>
+      <c r="D51" s="34"/>
       <c r="E51" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F51" s="14" t="s">
-        <v>10</v>
+      <c r="F51" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1773,15 +1785,15 @@
       <c r="B52" s="12">
         <v>44</v>
       </c>
-      <c r="C52" s="20" t="s">
+      <c r="C52" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="D52" s="21"/>
+      <c r="D52" s="23"/>
       <c r="E52" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F52" s="14" t="s">
-        <v>10</v>
+      <c r="F52" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1789,15 +1801,15 @@
       <c r="B53" s="12">
         <v>45</v>
       </c>
-      <c r="C53" s="20" t="s">
+      <c r="C53" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="D53" s="21"/>
+      <c r="D53" s="23"/>
       <c r="E53" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F53" s="14" t="s">
-        <v>10</v>
+      <c r="F53" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1805,15 +1817,15 @@
       <c r="B54" s="12">
         <v>46</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D54" s="21"/>
+      <c r="D54" s="23"/>
       <c r="E54" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F54" s="14" t="s">
-        <v>10</v>
+      <c r="F54" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1821,15 +1833,15 @@
       <c r="B55" s="12">
         <v>47</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D55" s="21"/>
+      <c r="D55" s="23"/>
       <c r="E55" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F55" s="14" t="s">
-        <v>10</v>
+      <c r="F55" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1837,15 +1849,15 @@
       <c r="B56" s="12">
         <v>48</v>
       </c>
-      <c r="C56" s="20" t="s">
+      <c r="C56" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="D56" s="21"/>
+      <c r="D56" s="23"/>
       <c r="E56" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F56" s="14" t="s">
-        <v>10</v>
+      <c r="F56" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1853,15 +1865,15 @@
       <c r="B57" s="12">
         <v>49</v>
       </c>
-      <c r="C57" s="20" t="s">
+      <c r="C57" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="D57" s="21"/>
+      <c r="D57" s="23"/>
       <c r="E57" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="F57" s="14" t="s">
-        <v>10</v>
+      <c r="F57" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1869,25 +1881,53 @@
       <c r="B58" s="19">
         <v>50</v>
       </c>
-      <c r="C58" s="34" t="s">
+      <c r="C58" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D58" s="35"/>
+      <c r="D58" s="21"/>
       <c r="E58" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F58" s="14" t="s">
-        <v>10</v>
+      <c r="F58" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="B2:F3"/>
     <mergeCell ref="C8:D8"/>
@@ -1900,40 +1940,12 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>